<commit_message>
December 22. Átalakítás 1
</commit_message>
<xml_diff>
--- a/MyDataGrid/Takarékos autók.xlsx
+++ b/MyDataGrid/Takarékos autók.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gmiskola-my.sharepoint.com/personal/kovacszsolt100_gmiskola_hu/Documents/Programozás/DotNetBackend2/MyDataGrid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EDD9948-7FCF-4FF8-9934-3D2E7E05F40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{5EDD9948-7FCF-4FF8-9934-3D2E7E05F40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F324EDD7-9FDA-48F1-9CD0-C01C9D3BA358}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF5E245A-700D-4E39-BE98-09EFC3E9A7CA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Helyezés</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Citroen C1 (982)</t>
+  </si>
+  <si>
+    <t>Dátum</t>
   </si>
 </sst>
 </file>
@@ -161,17 +164,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -187,6 +200,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -486,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C8469C-39AB-41DF-A9D4-2C85DC170C18}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,9 +514,10 @@
     <col min="1" max="1" width="9.21875" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.21875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -509,115 +527,148 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+      <c r="D2" s="7">
+        <v>38639</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="D3" s="7">
+        <v>38640</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="D4" s="7">
+        <v>38641</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="D5" s="7">
+        <v>38642</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="D6" s="7">
+        <v>38643</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="D7" s="7">
+        <v>38644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="D8" s="7">
+        <v>38645</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="D9" s="7">
+        <v>38646</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="4">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="D10" s="7">
+        <v>38647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>4.7</v>
+      </c>
+      <c r="D11" s="7">
+        <v>38648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>